<commit_message>
Refatorando artefatos 04,12,22 e 23. Artefatos 22,23 corrigidos em grupo
</commit_message>
<xml_diff>
--- a/artefatos/23 - Matrizes de Rastreabilidade (Características x SSS incompleto).xlsx
+++ b/artefatos/23 - Matrizes de Rastreabilidade (Características x SSS incompleto).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD77235-92D8-44FC-91CC-99F5FDA94277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6519E31B-8B9A-4E7C-80B0-EBA39AF86F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{687264DB-7704-40A5-AC63-81B79CD6956B}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="15375" windowHeight="7875" xr2:uid="{687264DB-7704-40A5-AC63-81B79CD6956B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>SSS 0001</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>SSS0009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caracteristicas </t>
+  </si>
+  <si>
+    <t>Cancelamento do pedido</t>
   </si>
 </sst>
 </file>
@@ -629,14 +635,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB563BAB-74BE-4A51-912A-1877866596D9}">
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,9 +833,15 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>

</xml_diff>

<commit_message>
Refactor artefato 22 e complementando o artefato 23
</commit_message>
<xml_diff>
--- a/artefatos/23 - Matrizes de Rastreabilidade (Características x SSS incompleto).xlsx
+++ b/artefatos/23 - Matrizes de Rastreabilidade (Características x SSS incompleto).xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Documents\MaapSystem\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6519E31B-8B9A-4E7C-80B0-EBA39AF86F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E262777-D274-4D34-965B-274F7D5829C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="690" windowWidth="15375" windowHeight="7875" xr2:uid="{687264DB-7704-40A5-AC63-81B79CD6956B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz de Rastreabilidade" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>SSS 0001</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SSS0006</t>
   </si>
   <si>
-    <t>car0009</t>
-  </si>
-  <si>
     <t>SSS0007</t>
   </si>
   <si>
@@ -84,10 +81,13 @@
     <t>SSS0009</t>
   </si>
   <si>
-    <t xml:space="preserve">Caracteristicas </t>
-  </si>
-  <si>
-    <t>Cancelamento do pedido</t>
+    <t>SSS0010</t>
+  </si>
+  <si>
+    <t>Car 0009</t>
+  </si>
+  <si>
+    <t>Car 0010</t>
   </si>
 </sst>
 </file>
@@ -131,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,17 +160,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -189,17 +178,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -258,11 +236,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,49 +269,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,51 +615,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB563BAB-74BE-4A51-912A-1877866596D9}">
-  <dimension ref="A2:J23"/>
+  <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="J2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
@@ -687,161 +672,169 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="I3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -851,7 +844,7 @@
       <c r="J13" s="1"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="19"/>
+      <c r="C23" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>